<commit_message>
update import function and db
</commit_message>
<xml_diff>
--- a/example_data/import/project_contents/fbq_sub_projects.xlsx
+++ b/example_data/import/project_contents/fbq_sub_projects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/44b92e2d6c7d28b1/TU Berlin neu/Masterarbeit/Code/pros/example_data/import/project_contents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{1EA36FC3-6BC3-DA47-B9B3-85C60DB4737B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{929085E7-A800-0545-BCCF-D8BA31F3BA61}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{1EA36FC3-6BC3-DA47-B9B3-85C60DB4737B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07FEBDC8-4752-7B46-B128-CEAB65BDFCF7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27420" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deutschlandtakt" sheetId="4" r:id="rId1"/>
@@ -20,8 +20,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="NKV &lt; 1,5" guid="{23E76F66-981C-4206-9E06-CBB72D7DAC5B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Noch nicht in qgis" guid="{88289622-D034-4E38-A0C0-61CEB0F9C67E}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="NKV &lt; 1,5" guid="{23E76F66-981C-4206-9E06-CBB72D7DAC5B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -546,9 +546,9 @@
   </sheetPr>
   <dimension ref="A1:AX170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA3" sqref="AA3"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -562,7 +562,7 @@
     <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="14.5" customWidth="1"/>
     <col min="11" max="11" width="10.1640625" customWidth="1"/>
-    <col min="12" max="12" width="6" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.33203125" customWidth="1"/>
     <col min="14" max="14" width="7.6640625" customWidth="1"/>
     <col min="15" max="15" width="8.83203125" customWidth="1"/>

</xml_diff>